<commit_message>
added changes UPH to putwall and regular pick
</commit_message>
<xml_diff>
--- a/output/processed_data.xlsx
+++ b/output/processed_data.xlsx
@@ -33,12 +33,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -53,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -438,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,17 +454,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>UserID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>PutwallPickingQuantity</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
@@ -466,248 +478,305 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABHI4088.ABHISHEK</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>286</v>
+        <v>197</v>
       </c>
       <c r="C2" t="n">
-        <v>44.8041775456919</v>
+        <v>44</v>
+      </c>
+      <c r="D2" t="n">
+        <v>268.64</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ANASTASIIA.MAKHTOUT</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="C3" t="n">
-        <v>1.879895561357702</v>
+        <v>91</v>
+      </c>
+      <c r="D3" t="n">
+        <v>181.98</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ANASTASIIA.MAKHTOUT</t>
+          <t>ABHI4088.ABHISHEK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="C4" t="n">
-        <v>43.23759791122715</v>
+        <v>104</v>
+      </c>
+      <c r="D4" t="n">
+        <v>165</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C5" t="n">
-        <v>27.10182767624021</v>
+        <v>67</v>
+      </c>
+      <c r="D5" t="n">
+        <v>151.34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="C6" t="n">
-        <v>7.206266318537859</v>
+        <v>76</v>
+      </c>
+      <c r="D6" t="n">
+        <v>136.58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>197</v>
+        <v>120</v>
       </c>
       <c r="C7" t="n">
-        <v>30.86161879895561</v>
+        <v>53</v>
+      </c>
+      <c r="D7" t="n">
+        <v>135.85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HARJ4282.SINGH</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>51</v>
+        <v>378</v>
       </c>
       <c r="C8" t="n">
-        <v>7.989556135770234</v>
+        <v>167</v>
+      </c>
+      <c r="D8" t="n">
+        <v>135.81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>169</v>
+        <v>94</v>
       </c>
       <c r="C9" t="n">
-        <v>26.47519582245431</v>
+        <v>46</v>
+      </c>
+      <c r="D9" t="n">
+        <v>122.61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>351</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1566579634464752</v>
+        <v>182</v>
+      </c>
+      <c r="D10" t="n">
+        <v>115.71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="C11" t="n">
-        <v>18.79895561357702</v>
+        <v>88</v>
+      </c>
+      <c r="D11" t="n">
+        <v>96.14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MDSAIFUL.ISLAM</t>
+          <t>RAVI4279.THAKUR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C12" t="n">
-        <v>10.33942558746736</v>
+        <v>10</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>7.676240208877284</v>
+        <v>6</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>MDSAIFUL.ISLAM</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="C14" t="n">
-        <v>0.4699738903394255</v>
+        <v>19</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>RAVI4279.THAKUR</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
-        <v>4.543080939947781</v>
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SEPIDEH.AZARIHASHJIN</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C16" t="n">
-        <v>3.759791122715404</v>
+        <v>18</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="C17" t="n">
-        <v>14.72584856396867</v>
+        <v>19</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>378</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>59.21671018276762</v>
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>HARJ4282.SINGH</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>351</v>
+        <v>51</v>
       </c>
       <c r="C19" t="n">
-        <v>54.98694516971279</v>
+        <v>17</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="C20" t="n">
-        <v>22.088772845953</v>
+        <v>15</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -720,7 +789,22 @@
         <v>39</v>
       </c>
       <c r="C21" t="n">
-        <v>6.109660574412533</v>
+        <v>9</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Average UPH</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr"/>
+      <c r="C22" s="1" t="inlineStr"/>
+      <c r="D22" s="1" t="n">
+        <v>150.97</v>
       </c>
     </row>
   </sheetData>
@@ -734,7 +818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,17 +827,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>UserID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>RegularPickQuantity</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
@@ -762,300 +851,369 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="C2" t="n">
-        <v>1.253263707571801</v>
+        <v>38</v>
+      </c>
+      <c r="D2" t="n">
+        <v>282.63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANASTASIIA.MAKHTOUT</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>148</v>
       </c>
       <c r="C3" t="n">
-        <v>2.663185378590078</v>
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
+        <v>80.73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ARJUNBHAI.PATEL</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>4.22976501305483</v>
+        <v>43</v>
+      </c>
+      <c r="D4" t="n">
+        <v>30.7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>23.18537859007833</v>
+        <v>34</v>
+      </c>
+      <c r="D5" t="n">
+        <v>24.71</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1566579634464752</v>
+        <v>3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>179</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>28.04177545691906</v>
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HARJ4282.SINGH</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3133159268929503</v>
+        <v>19</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7832898172323759</v>
+        <v>22</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1566579634464752</v>
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1566579634464752</v>
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1566579634464752</v>
+        <v>20</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>RAVI4279.THAKUR</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>5.483028720626631</v>
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C14" t="n">
-        <v>2.663185378590078</v>
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7832898172323759</v>
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>ANASTASIIA.MAKHTOUT</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16" t="n">
-        <v>3.133159268929504</v>
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RAVI4279.THAKUR</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3133159268929503</v>
+        <v>23</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SEPIDEH.AZARIHASHJIN</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>2.193211488250653</v>
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>KHINEHAYMAR.THAUNG</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>2.819843342036553</v>
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3133159268929503</v>
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3133159268929503</v>
+        <v>3</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>HARJ4282.SINGH</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>2.663185378590078</v>
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>3.446475195822454</v>
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C24" t="n">
-        <v>2.663185378590078</v>
+        <v>7</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1068,7 +1226,22 @@
         <v>9</v>
       </c>
       <c r="C25" t="n">
-        <v>1.409921671018277</v>
+        <v>12</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Average UPH</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr"/>
+      <c r="C26" s="1" t="inlineStr"/>
+      <c r="D26" s="1" t="n">
+        <v>104.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>